<commit_message>
appeal module initial setup with add and get timeline
</commit_message>
<xml_diff>
--- a/public/properties/Woodmere.xlsx
+++ b/public/properties/Woodmere.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hamza_SPS_Data\Projects\AOTC\Atrifacts\Property List\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="1485" windowWidth="24720" windowHeight="15180"/>
+    <workbookView xWindow="6300" yWindow="1485" windowWidth="24720" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -524,23 +524,23 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="3"/>
-    <cellStyle name="Comma 3" xfId="4"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal_PropPort" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal_PropPort" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
@@ -841,7 +841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
@@ -879,34 +879,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="30">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="56"/>
@@ -1096,118 +1096,118 @@
       <c r="G7" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="107">
+      <c r="H7" s="108">
         <v>1987</v>
       </c>
       <c r="I7" s="69">
         <v>2015</v>
       </c>
       <c r="J7" s="69"/>
-      <c r="K7" s="107" t="s">
+      <c r="K7" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="107">
+      <c r="L7" s="108">
         <v>16183636</v>
       </c>
-      <c r="M7" s="107">
+      <c r="M7" s="108">
         <v>392</v>
       </c>
-      <c r="N7" s="110">
+      <c r="N7" s="111">
         <v>3</v>
       </c>
-      <c r="O7" s="107">
+      <c r="O7" s="108">
         <v>42</v>
       </c>
-      <c r="P7" s="107" t="s">
+      <c r="P7" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="107" t="s">
+      <c r="Q7" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="R7" s="107" t="s">
+      <c r="R7" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="109">
+      <c r="S7" s="110">
         <v>2018</v>
       </c>
       <c r="T7" s="68" t="s">
         <v>24</v>
       </c>
       <c r="U7" s="72"/>
-      <c r="V7" s="107">
+      <c r="V7" s="108">
         <v>61750</v>
       </c>
       <c r="W7" s="68" t="s">
         <v>12</v>
       </c>
       <c r="X7" s="74"/>
-      <c r="Y7" s="107" t="s">
+      <c r="Y7" s="108" t="s">
         <v>34</v>
       </c>
       <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" s="15" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="108" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="19">
         <v>21046</v>
       </c>
-      <c r="C8" s="107">
+      <c r="C8" s="108">
         <v>72788</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="107" t="s">
+      <c r="G8" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="107">
+      <c r="H8" s="108">
         <v>1987</v>
       </c>
       <c r="I8" s="20">
         <v>2015</v>
       </c>
       <c r="J8" s="20"/>
-      <c r="K8" s="107" t="s">
+      <c r="K8" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="107">
+      <c r="L8" s="108">
         <v>16072788</v>
       </c>
-      <c r="M8" s="107">
+      <c r="M8" s="108">
         <v>392</v>
       </c>
-      <c r="N8" s="107">
+      <c r="N8" s="108">
         <v>3</v>
       </c>
-      <c r="O8" s="108">
+      <c r="O8" s="109">
         <v>42</v>
       </c>
-      <c r="P8" s="107" t="s">
+      <c r="P8" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="107" t="s">
+      <c r="Q8" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="107" t="s">
+      <c r="R8" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="109">
+      <c r="S8" s="110">
         <v>2018</v>
       </c>
       <c r="T8" s="68" t="s">
         <v>24</v>
       </c>
       <c r="U8" s="20"/>
-      <c r="V8" s="107">
+      <c r="V8" s="108">
         <v>62379</v>
       </c>
       <c r="W8" s="68" t="s">
         <v>12</v>
       </c>
       <c r="X8" s="19"/>
-      <c r="Y8" s="107" t="s">
+      <c r="Y8" s="108" t="s">
         <v>34</v>
       </c>
       <c r="Z8" s="27"/>

</xml_diff>

<commit_message>
resolved issue of jurisdiction repitition
</commit_message>
<xml_diff>
--- a/public/properties/Woodmere.xlsx
+++ b/public/properties/Woodmere.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hamza_SPS_Data\Projects\AOTC\Atrifacts\Property List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7797131-9571-4489-A13B-15EFF9621F9F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395A662-B9D1-491C-9924-02D8B29AC0AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6300" yWindow="1485" windowWidth="24720" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>REVAL Year</t>
     <phoneticPr fontId="9" type="noConversion"/>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>9891 Broken Land Pkwy., Columbia, MD 21046</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>Maryland</t>
   </si>
 </sst>
 </file>
@@ -830,8 +836,8 @@
   </sheetPr>
   <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="25" zoomScalePageLayoutView="53" workbookViewId="0">
-      <selection activeCell="R7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="25" zoomScalePageLayoutView="53" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="15"/>
@@ -839,8 +845,9 @@
     <col min="1" max="1" width="12.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="105" customWidth="1"/>
-    <col min="4" max="4" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1004,7 +1011,9 @@
       <c r="D6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
         <v>23</v>
@@ -1102,7 +1111,9 @@
         <v>72788</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="E8" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="20"/>
       <c r="G8" s="107" t="s">
         <v>30</v>

</xml_diff>